<commit_message>
Added APR reason category and one list with APR
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/reason_list.xlsx
+++ b/mosip_master/xlsx/reason_list.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nira_dev\mosip-data\mosip_master\xlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC532618-1835-427F-BF04-1E1E646A0D43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,197 +25,199 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="60">
-  <si>
-    <t xml:space="preserve">lang_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">descr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rsncat_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_active</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age-Photo Mismatch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mismatch between the Age and Photo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gender-Photo Mismatch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gender-Photo Mismatch between Gender and Photo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IAD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invalid Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invalid Address found</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DPG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duplicate Registration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duplicate Registration found</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OTH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Others</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All the Details are matching</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All the Demographic Details are Matching</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Only the Photograph is Matching</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Some of the Demographic Details are Matching</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Décalage de lâge-Photo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Discordance entre lâge et la Photo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incompatibilité de sexe-Photo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sexe-Photo discordance entre le sexe et la Photo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adresse non valide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adresse non valide trouvée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enregistrement en double</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Double enregistrement trouvé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dautres</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tous les détails sont adaptent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tous les détails démographiques sont Matching</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La photographie est le rapprochement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Certains détails démographiques sont Matching</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ara</t>
-  </si>
-  <si>
-    <t xml:space="preserve">عدم تطابق الصورة مع العمر</t>
-  </si>
-  <si>
-    <t xml:space="preserve">عدم التطابق بين العمر والصورة</t>
-  </si>
-  <si>
-    <t xml:space="preserve">عدم تطابق الصورة بين الجنسين</t>
-  </si>
-  <si>
-    <t xml:space="preserve">عدم تطابق الصورة بين الجنسين والصورة</t>
-  </si>
-  <si>
-    <t xml:space="preserve">عنوان خاطئ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">تم العثور على عنوان غير صالح</t>
-  </si>
-  <si>
-    <t xml:space="preserve">تسجيل مكرر</t>
-  </si>
-  <si>
-    <t xml:space="preserve">تم العثور على تسجيل مكرر</t>
-  </si>
-  <si>
-    <t xml:space="preserve">آحرون</t>
-  </si>
-  <si>
-    <t xml:space="preserve">كل التفاصيل متطابقة</t>
-  </si>
-  <si>
-    <t xml:space="preserve">جميع التفاصيل الديموغرافية متطابقة</t>
-  </si>
-  <si>
-    <t xml:space="preserve">فقط الصورة هي المطابقة</t>
-  </si>
-  <si>
-    <t xml:space="preserve">بعض التفاصيل الديموغرافية متطابقة</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="62">
+  <si>
+    <t>lang_code</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>descr</t>
+  </si>
+  <si>
+    <t>rsncat_code</t>
+  </si>
+  <si>
+    <t>is_active</t>
+  </si>
+  <si>
+    <t>eng</t>
+  </si>
+  <si>
+    <t>APM</t>
+  </si>
+  <si>
+    <t>Age-Photo Mismatch</t>
+  </si>
+  <si>
+    <t>Mismatch between the Age and Photo</t>
+  </si>
+  <si>
+    <t>CLR</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>GPM</t>
+  </si>
+  <si>
+    <t>Gender-Photo Mismatch</t>
+  </si>
+  <si>
+    <t>Gender-Photo Mismatch between Gender and Photo</t>
+  </si>
+  <si>
+    <t>IAD</t>
+  </si>
+  <si>
+    <t>Invalid Address</t>
+  </si>
+  <si>
+    <t>Invalid Address found</t>
+  </si>
+  <si>
+    <t>DPG</t>
+  </si>
+  <si>
+    <t>Duplicate Registration</t>
+  </si>
+  <si>
+    <t>Duplicate Registration found</t>
+  </si>
+  <si>
+    <t>OTH</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>ADM</t>
+  </si>
+  <si>
+    <t>All the Details are matching</t>
+  </si>
+  <si>
+    <t>MNA</t>
+  </si>
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>All the Demographic Details are Matching</t>
+  </si>
+  <si>
+    <t>OPM</t>
+  </si>
+  <si>
+    <t>Only the Photograph is Matching</t>
+  </si>
+  <si>
+    <t>SDM</t>
+  </si>
+  <si>
+    <t>Some of the Demographic Details are Matching</t>
+  </si>
+  <si>
+    <t>fra</t>
+  </si>
+  <si>
+    <t>Décalage de lâge-Photo</t>
+  </si>
+  <si>
+    <t>Discordance entre lâge et la Photo</t>
+  </si>
+  <si>
+    <t>Incompatibilité de sexe-Photo</t>
+  </si>
+  <si>
+    <t>Sexe-Photo discordance entre le sexe et la Photo</t>
+  </si>
+  <si>
+    <t>Adresse non valide</t>
+  </si>
+  <si>
+    <t>Adresse non valide trouvée</t>
+  </si>
+  <si>
+    <t>Enregistrement en double</t>
+  </si>
+  <si>
+    <t>Double enregistrement trouvé</t>
+  </si>
+  <si>
+    <t>Dautres</t>
+  </si>
+  <si>
+    <t>Tous les détails sont adaptent</t>
+  </si>
+  <si>
+    <t>Tous les détails démographiques sont Matching</t>
+  </si>
+  <si>
+    <t>La photographie est le rapprochement</t>
+  </si>
+  <si>
+    <t>Certains détails démographiques sont Matching</t>
+  </si>
+  <si>
+    <t>ara</t>
+  </si>
+  <si>
+    <t>عدم تطابق الصورة مع العمر</t>
+  </si>
+  <si>
+    <t>عدم التطابق بين العمر والصورة</t>
+  </si>
+  <si>
+    <t>عدم تطابق الصورة بين الجنسين</t>
+  </si>
+  <si>
+    <t>عدم تطابق الصورة بين الجنسين والصورة</t>
+  </si>
+  <si>
+    <t>عنوان خاطئ</t>
+  </si>
+  <si>
+    <t>تم العثور على عنوان غير صالح</t>
+  </si>
+  <si>
+    <t>تسجيل مكرر</t>
+  </si>
+  <si>
+    <t>تم العثور على تسجيل مكرر</t>
+  </si>
+  <si>
+    <t>آحرون</t>
+  </si>
+  <si>
+    <t>كل التفاصيل متطابقة</t>
+  </si>
+  <si>
+    <t>جميع التفاصيل الديموغرافية متطابقة</t>
+  </si>
+  <si>
+    <t>فقط الصورة هي المطابقة</t>
+  </si>
+  <si>
+    <t>بعض التفاصيل الديموغرافية متطابقة</t>
+  </si>
+  <si>
+    <t>ATDM</t>
+  </si>
+  <si>
+    <t>APR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -219,25 +226,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <name val="Cambria"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -250,102 +241,373 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20:D28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="46.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.43"/>
+    <col min="3" max="3" width="48.85546875" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -365,7 +627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -385,7 +647,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -405,7 +667,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -425,7 +687,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -445,7 +707,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -459,13 +721,13 @@
         <v>22</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -485,7 +747,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -505,7 +767,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -525,7 +787,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -545,7 +807,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>32</v>
       </c>
@@ -565,7 +827,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>32</v>
       </c>
@@ -585,7 +847,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
@@ -605,7 +867,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -625,7 +887,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>32</v>
       </c>
@@ -639,13 +901,13 @@
         <v>41</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>32</v>
       </c>
@@ -665,7 +927,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
@@ -685,7 +947,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>32</v>
       </c>
@@ -705,7 +967,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>32</v>
       </c>
@@ -725,7 +987,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>46</v>
       </c>
@@ -745,7 +1007,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>46</v>
       </c>
@@ -765,7 +1027,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>46</v>
       </c>
@@ -785,7 +1047,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>46</v>
       </c>
@@ -805,7 +1067,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>46</v>
       </c>
@@ -819,13 +1081,13 @@
         <v>55</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>46</v>
       </c>
@@ -845,7 +1107,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>46</v>
       </c>
@@ -865,7 +1127,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>46</v>
       </c>
@@ -885,7 +1147,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>46</v>
       </c>
@@ -905,14 +1167,28 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>